<commit_message>
Updated to include Titles!!!
</commit_message>
<xml_diff>
--- a/SasquatchCAIRS/SasquatchCAIRS/ReportTemplate.xlsx
+++ b/SasquatchCAIRS/SasquatchCAIRS/ReportTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="19440" windowHeight="8190" tabRatio="704"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -109,7 +109,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -118,7 +118,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$D$2</c:f>
+              <c:f>Sheet1!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -131,7 +131,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -140,7 +140,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:f>Sheet1!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -149,7 +149,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$D$3</c:f>
+              <c:f>Sheet1!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -166,11 +166,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168243200"/>
-        <c:axId val="168244736"/>
+        <c:axId val="92962816"/>
+        <c:axId val="92964352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168243200"/>
+        <c:axId val="92962816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -180,7 +180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168244736"/>
+        <c:crossAx val="92964352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -188,7 +188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168244736"/>
+        <c:axId val="92964352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -199,7 +199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168243200"/>
+        <c:crossAx val="92962816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -247,7 +247,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet10!$A$2</c:f>
+              <c:f>Sheet10!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -256,7 +256,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet10!$B$1:$D$1</c:f>
+              <c:f>Sheet10!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -265,7 +265,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet10!$B$2:$D$2</c:f>
+              <c:f>Sheet10!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -278,7 +278,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet10!$A$3</c:f>
+              <c:f>Sheet10!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -287,7 +287,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet10!$B$1:$D$1</c:f>
+              <c:f>Sheet10!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -296,7 +296,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet10!$B$3:$D$3</c:f>
+              <c:f>Sheet10!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -313,11 +313,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171062400"/>
-        <c:axId val="171063936"/>
+        <c:axId val="99714176"/>
+        <c:axId val="99715712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171062400"/>
+        <c:axId val="99714176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171063936"/>
+        <c:crossAx val="99715712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -335,7 +335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171063936"/>
+        <c:axId val="99715712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,7 +346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171062400"/>
+        <c:crossAx val="99714176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -393,7 +393,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet11!$A$2</c:f>
+              <c:f>Sheet11!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -402,7 +402,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet11!$B$1:$D$1</c:f>
+              <c:f>Sheet11!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -411,7 +411,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet11!$B$2:$D$2</c:f>
+              <c:f>Sheet11!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -424,7 +424,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet11!$A$3</c:f>
+              <c:f>Sheet11!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -433,7 +433,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet11!$B$1:$D$1</c:f>
+              <c:f>Sheet11!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -442,7 +442,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet11!$B$3:$D$3</c:f>
+              <c:f>Sheet11!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -459,11 +459,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171101568"/>
-        <c:axId val="171107456"/>
+        <c:axId val="100019584"/>
+        <c:axId val="100025472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171101568"/>
+        <c:axId val="100019584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -473,7 +473,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171107456"/>
+        <c:crossAx val="100025472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -481,7 +481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171107456"/>
+        <c:axId val="100025472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171101568"/>
+        <c:crossAx val="100019584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -539,7 +539,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet12!$A$2</c:f>
+              <c:f>Sheet12!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -548,7 +548,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet12!$B$1:$D$1</c:f>
+              <c:f>Sheet12!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -557,7 +557,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet12!$B$2:$D$2</c:f>
+              <c:f>Sheet12!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -570,7 +570,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet12!$A$3</c:f>
+              <c:f>Sheet12!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -579,7 +579,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet12!$B$1:$D$1</c:f>
+              <c:f>Sheet12!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -588,7 +588,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet12!$B$3:$D$3</c:f>
+              <c:f>Sheet12!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -605,11 +605,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171169664"/>
-        <c:axId val="171171200"/>
+        <c:axId val="99768192"/>
+        <c:axId val="99769728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171169664"/>
+        <c:axId val="99768192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +619,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171171200"/>
+        <c:crossAx val="99769728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -627,7 +627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171171200"/>
+        <c:axId val="99769728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171169664"/>
+        <c:crossAx val="99768192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -685,7 +685,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet13!$A$2</c:f>
+              <c:f>Sheet13!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -694,7 +694,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet13!$B$1:$D$1</c:f>
+              <c:f>Sheet13!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -703,7 +703,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet13!$B$2:$D$2</c:f>
+              <c:f>Sheet13!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -716,7 +716,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet13!$A$3</c:f>
+              <c:f>Sheet13!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -725,7 +725,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet13!$B$1:$D$1</c:f>
+              <c:f>Sheet13!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -734,7 +734,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet13!$B$3:$D$3</c:f>
+              <c:f>Sheet13!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -751,11 +751,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171286912"/>
-        <c:axId val="171288448"/>
+        <c:axId val="99807616"/>
+        <c:axId val="99809152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171286912"/>
+        <c:axId val="99807616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,7 +765,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171288448"/>
+        <c:crossAx val="99809152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -773,7 +773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171288448"/>
+        <c:axId val="99809152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +784,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171286912"/>
+        <c:crossAx val="99807616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -831,7 +831,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet14!$A$2</c:f>
+              <c:f>Sheet14!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -840,7 +840,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet14!$B$1:$D$1</c:f>
+              <c:f>Sheet14!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -849,7 +849,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet14!$B$2:$D$2</c:f>
+              <c:f>Sheet14!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -862,7 +862,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet14!$A$3</c:f>
+              <c:f>Sheet14!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -871,7 +871,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet14!$B$1:$D$1</c:f>
+              <c:f>Sheet14!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -880,7 +880,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet14!$B$3:$D$3</c:f>
+              <c:f>Sheet14!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -897,11 +897,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171358848"/>
-        <c:axId val="171360640"/>
+        <c:axId val="99953280"/>
+        <c:axId val="99955072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171358848"/>
+        <c:axId val="99953280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +911,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171360640"/>
+        <c:crossAx val="99955072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -919,7 +919,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171360640"/>
+        <c:axId val="99955072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171358848"/>
+        <c:crossAx val="99953280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -977,7 +977,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet15!$A$2</c:f>
+              <c:f>Sheet15!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -986,7 +986,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet15!$B$1:$D$1</c:f>
+              <c:f>Sheet15!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -995,7 +995,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet15!$B$2:$D$2</c:f>
+              <c:f>Sheet15!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1008,7 +1008,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet15!$A$3</c:f>
+              <c:f>Sheet15!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1017,7 +1017,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet15!$B$1:$D$1</c:f>
+              <c:f>Sheet15!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1026,7 +1026,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet15!$B$3:$D$3</c:f>
+              <c:f>Sheet15!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1043,11 +1043,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171648128"/>
-        <c:axId val="171649664"/>
+        <c:axId val="99980416"/>
+        <c:axId val="99981952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171648128"/>
+        <c:axId val="99980416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1057,7 +1057,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171649664"/>
+        <c:crossAx val="99981952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1065,7 +1065,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171649664"/>
+        <c:axId val="99981952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,14 +1076,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171648128"/>
+        <c:crossAx val="99980416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1124,7 +1123,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$2</c:f>
+              <c:f>Sheet2!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1133,7 +1132,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$B$1:$D$1</c:f>
+              <c:f>Sheet2!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1142,7 +1141,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$D$2</c:f>
+              <c:f>Sheet2!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1155,7 +1154,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$3</c:f>
+              <c:f>Sheet2!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1164,7 +1163,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$B$1:$D$1</c:f>
+              <c:f>Sheet2!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1173,7 +1172,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$D$3</c:f>
+              <c:f>Sheet2!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1190,11 +1189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="169822464"/>
-        <c:axId val="169824256"/>
+        <c:axId val="92911872"/>
+        <c:axId val="92913664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169822464"/>
+        <c:axId val="92911872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,7 +1203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169824256"/>
+        <c:crossAx val="92913664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1212,7 +1211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169824256"/>
+        <c:axId val="92913664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,7 +1222,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169822464"/>
+        <c:crossAx val="92911872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1270,7 +1269,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$2</c:f>
+              <c:f>Sheet3!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1279,7 +1278,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet3!$B$1:$D$1</c:f>
+              <c:f>Sheet3!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1288,7 +1287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$D$2</c:f>
+              <c:f>Sheet3!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1301,7 +1300,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$A$3</c:f>
+              <c:f>Sheet3!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1310,7 +1309,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet3!$B$1:$D$1</c:f>
+              <c:f>Sheet3!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1319,7 +1318,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$3:$D$3</c:f>
+              <c:f>Sheet3!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1336,11 +1335,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170459904"/>
-        <c:axId val="170461440"/>
+        <c:axId val="93348608"/>
+        <c:axId val="93350144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170459904"/>
+        <c:axId val="93348608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170461440"/>
+        <c:crossAx val="93350144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +1357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170461440"/>
+        <c:axId val="93350144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +1368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170459904"/>
+        <c:crossAx val="93348608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1416,7 +1415,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$A$2</c:f>
+              <c:f>Sheet4!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1425,7 +1424,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet4!$B$1:$D$1</c:f>
+              <c:f>Sheet4!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1434,7 +1433,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$2:$D$2</c:f>
+              <c:f>Sheet4!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1447,7 +1446,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet4!$A$3</c:f>
+              <c:f>Sheet4!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1456,7 +1455,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet4!$B$1:$D$1</c:f>
+              <c:f>Sheet4!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1465,7 +1464,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet4!$B$3:$D$3</c:f>
+              <c:f>Sheet4!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1482,11 +1481,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170511360"/>
-        <c:axId val="170525440"/>
+        <c:axId val="93469696"/>
+        <c:axId val="93475584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170511360"/>
+        <c:axId val="93469696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,7 +1495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170525440"/>
+        <c:crossAx val="93475584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1504,7 +1503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170525440"/>
+        <c:axId val="93475584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1515,7 +1514,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170511360"/>
+        <c:crossAx val="93469696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1562,7 +1561,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$A$2</c:f>
+              <c:f>Sheet5!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1571,7 +1570,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet5!$B$1:$D$1</c:f>
+              <c:f>Sheet5!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1580,7 +1579,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$2:$D$2</c:f>
+              <c:f>Sheet5!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1593,7 +1592,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$A$3</c:f>
+              <c:f>Sheet5!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1602,7 +1601,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet5!$B$1:$D$1</c:f>
+              <c:f>Sheet5!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1611,7 +1610,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$3:$D$3</c:f>
+              <c:f>Sheet5!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1628,11 +1627,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170568320"/>
-        <c:axId val="170578304"/>
+        <c:axId val="94833280"/>
+        <c:axId val="94843264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170568320"/>
+        <c:axId val="94833280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170578304"/>
+        <c:crossAx val="94843264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1650,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170578304"/>
+        <c:axId val="94843264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,13 +1660,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170568320"/>
+        <c:crossAx val="94833280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1708,7 +1708,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$A$2</c:f>
+              <c:f>Sheet6!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1717,7 +1717,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet6!$B$1:$D$1</c:f>
+              <c:f>Sheet6!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1726,7 +1726,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$B$2:$D$2</c:f>
+              <c:f>Sheet6!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1739,7 +1739,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet6!$A$3</c:f>
+              <c:f>Sheet6!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1748,7 +1748,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet6!$B$1:$D$1</c:f>
+              <c:f>Sheet6!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1757,7 +1757,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet6!$B$3:$D$3</c:f>
+              <c:f>Sheet6!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1774,11 +1774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170640896"/>
-        <c:axId val="170642432"/>
+        <c:axId val="94909952"/>
+        <c:axId val="94911488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170640896"/>
+        <c:axId val="94909952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1788,7 +1788,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170642432"/>
+        <c:crossAx val="94911488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1796,7 +1796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170642432"/>
+        <c:axId val="94911488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +1807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170640896"/>
+        <c:crossAx val="94909952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1854,7 +1854,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet7!$A$2</c:f>
+              <c:f>Sheet7!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1863,7 +1863,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet7!$B$1:$D$1</c:f>
+              <c:f>Sheet7!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1872,7 +1872,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet7!$B$2:$D$2</c:f>
+              <c:f>Sheet7!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1885,7 +1885,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet7!$A$3</c:f>
+              <c:f>Sheet7!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1894,7 +1894,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet7!$B$1:$D$1</c:f>
+              <c:f>Sheet7!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1903,7 +1903,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet7!$B$3:$D$3</c:f>
+              <c:f>Sheet7!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1920,11 +1920,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170680320"/>
-        <c:axId val="170681856"/>
+        <c:axId val="94945280"/>
+        <c:axId val="94946816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170680320"/>
+        <c:axId val="94945280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1934,7 +1934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170681856"/>
+        <c:crossAx val="94946816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1942,7 +1942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170681856"/>
+        <c:axId val="94946816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,7 +1953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170680320"/>
+        <c:crossAx val="94945280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2000,7 +2000,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet8!$A$2</c:f>
+              <c:f>Sheet8!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -2009,7 +2009,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet8!$B$1:$D$1</c:f>
+              <c:f>Sheet8!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2018,7 +2018,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet8!$B$2:$D$2</c:f>
+              <c:f>Sheet8!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2031,7 +2031,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet8!$A$3</c:f>
+              <c:f>Sheet8!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -2040,7 +2040,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet8!$B$1:$D$1</c:f>
+              <c:f>Sheet8!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2049,7 +2049,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet8!$B$3:$D$3</c:f>
+              <c:f>Sheet8!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2066,11 +2066,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170942848"/>
-        <c:axId val="170944384"/>
+        <c:axId val="99602816"/>
+        <c:axId val="99604352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170942848"/>
+        <c:axId val="99602816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,7 +2080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170944384"/>
+        <c:crossAx val="99604352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2088,7 +2088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170944384"/>
+        <c:axId val="99604352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2099,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170942848"/>
+        <c:crossAx val="99602816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2146,7 +2146,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet9!$A$2</c:f>
+              <c:f>Sheet9!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -2155,7 +2155,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet9!$B$1:$D$1</c:f>
+              <c:f>Sheet9!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2164,7 +2164,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet9!$B$2:$D$2</c:f>
+              <c:f>Sheet9!$B$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2177,7 +2177,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet9!$A$3</c:f>
+              <c:f>Sheet9!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -2186,7 +2186,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet9!$B$1:$D$1</c:f>
+              <c:f>Sheet9!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2195,7 +2195,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet9!$B$3:$D$3</c:f>
+              <c:f>Sheet9!$B$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2212,11 +2212,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="170986112"/>
-        <c:axId val="171004288"/>
+        <c:axId val="99641984"/>
+        <c:axId val="99656064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170986112"/>
+        <c:axId val="99641984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,7 +2226,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171004288"/>
+        <c:crossAx val="99656064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2234,7 +2234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171004288"/>
+        <c:axId val="99656064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2245,7 +2245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170986112"/>
+        <c:crossAx val="99641984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2270,16 +2270,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2563,7 +2563,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2773,7 +2773,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>

</xml_diff>